<commit_message>
readme.md and some other changes
</commit_message>
<xml_diff>
--- a/etl/source/metadata.xlsx
+++ b/etl/source/metadata.xlsx
@@ -15,7 +15,7 @@
     <sheet name="metadata" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">metadata!$A$1:$E$78</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">metadata!$A$1:$E$80</definedName>
   </definedNames>
   <calcPr calcId="0" concurrentCalc="0"/>
   <extLst>
@@ -254,9 +254,6 @@
     <t>WPP2015_POP_F10_2_FEMINITY_RATIO_BY_BROAD_AGE_GROUP.XLS</t>
   </si>
   <si>
-    <t>FeminityRato_FemalePer100Male</t>
-  </si>
-  <si>
     <t>WPP2015_POP_F15_1_ANNUAL_POPULATION_BY_AGE_BOTH_SEXES.XLS</t>
   </si>
   <si>
@@ -705,6 +702,9 @@
   </si>
   <si>
     <t>ddf--datapoints--LifeExpectancy--by--ref_area_code--year--variant--age1yearinterval--gender--freq</t>
+  </si>
+  <si>
+    <t>FeminityRatio_FemalePer100Male</t>
   </si>
 </sst>
 </file>
@@ -1061,7 +1061,7 @@
   <dimension ref="A1:E80"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1091,41 +1091,41 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>5</v>
+        <v>80</v>
       </c>
       <c r="B2" t="s">
-        <v>6</v>
+        <v>76</v>
       </c>
       <c r="C2" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="D2" t="s">
-        <v>8</v>
+        <v>81</v>
       </c>
       <c r="E2" t="s">
-        <v>175</v>
+        <v>121</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>187</v>
+        <v>27</v>
       </c>
       <c r="B3" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="1" t="s">
-        <v>9</v>
+      <c r="C3" t="s">
+        <v>11</v>
       </c>
       <c r="D3" t="s">
-        <v>8</v>
+        <v>28</v>
       </c>
       <c r="E3" t="s">
-        <v>174</v>
+        <v>164</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>10</v>
+        <v>29</v>
       </c>
       <c r="B4" t="s">
         <v>6</v>
@@ -1134,15 +1134,15 @@
         <v>11</v>
       </c>
       <c r="D4" t="s">
-        <v>12</v>
+        <v>30</v>
       </c>
       <c r="E4" t="s">
-        <v>173</v>
+        <v>163</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>13</v>
+        <v>31</v>
       </c>
       <c r="B5" t="s">
         <v>6</v>
@@ -1151,15 +1151,15 @@
         <v>11</v>
       </c>
       <c r="D5" t="s">
-        <v>14</v>
+        <v>32</v>
       </c>
       <c r="E5" t="s">
-        <v>172</v>
+        <v>162</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>15</v>
+        <v>33</v>
       </c>
       <c r="B6" t="s">
         <v>6</v>
@@ -1168,15 +1168,15 @@
         <v>11</v>
       </c>
       <c r="D6" t="s">
-        <v>16</v>
+        <v>34</v>
       </c>
       <c r="E6" t="s">
-        <v>171</v>
+        <v>161</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>17</v>
+        <v>35</v>
       </c>
       <c r="B7" t="s">
         <v>6</v>
@@ -1185,32 +1185,32 @@
         <v>11</v>
       </c>
       <c r="D7" t="s">
-        <v>18</v>
+        <v>36</v>
       </c>
       <c r="E7" t="s">
-        <v>170</v>
+        <v>160</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>19</v>
+        <v>96</v>
       </c>
       <c r="B8" t="s">
-        <v>6</v>
+        <v>76</v>
       </c>
       <c r="C8" t="s">
         <v>11</v>
       </c>
       <c r="D8" t="s">
-        <v>20</v>
+        <v>97</v>
       </c>
       <c r="E8" t="s">
-        <v>169</v>
+        <v>129</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="B9" t="s">
         <v>6</v>
@@ -1219,15 +1219,15 @@
         <v>11</v>
       </c>
       <c r="D9" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="E9" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B10" t="s">
         <v>6</v>
@@ -1236,15 +1236,15 @@
         <v>11</v>
       </c>
       <c r="D10" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="E10" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="B11" t="s">
         <v>6</v>
@@ -1253,15 +1253,15 @@
         <v>11</v>
       </c>
       <c r="D11" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="E11" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="B12" t="s">
         <v>6</v>
@@ -1270,15 +1270,15 @@
         <v>11</v>
       </c>
       <c r="D12" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="E12" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="B13" t="s">
         <v>6</v>
@@ -1287,536 +1287,542 @@
         <v>11</v>
       </c>
       <c r="D13" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="E13" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>31</v>
+        <v>73</v>
       </c>
       <c r="B14" t="s">
-        <v>6</v>
+        <v>58</v>
       </c>
       <c r="C14" t="s">
         <v>11</v>
       </c>
       <c r="D14" t="s">
-        <v>32</v>
+        <v>224</v>
       </c>
       <c r="E14" t="s">
-        <v>163</v>
+        <v>217</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>33</v>
+        <v>60</v>
       </c>
       <c r="B15" t="s">
-        <v>6</v>
+        <v>190</v>
       </c>
       <c r="C15" t="s">
         <v>11</v>
       </c>
       <c r="D15" t="s">
-        <v>34</v>
+        <v>61</v>
       </c>
       <c r="E15" t="s">
-        <v>162</v>
+        <v>204</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>35</v>
+        <v>92</v>
       </c>
       <c r="B16" t="s">
-        <v>6</v>
+        <v>76</v>
       </c>
       <c r="C16" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="D16" t="s">
-        <v>36</v>
+        <v>93</v>
       </c>
       <c r="E16" t="s">
-        <v>161</v>
+        <v>127</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>37</v>
-      </c>
-      <c r="B17" t="s">
-        <v>6</v>
-      </c>
-      <c r="C17" t="s">
-        <v>11</v>
+        <v>189</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>9</v>
       </c>
       <c r="D17" t="s">
-        <v>38</v>
+        <v>69</v>
       </c>
       <c r="E17" t="s">
-        <v>160</v>
+        <v>223</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>39</v>
-      </c>
-      <c r="B18" t="s">
-        <v>6</v>
+        <v>68</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>190</v>
       </c>
       <c r="C18" t="s">
-        <v>11</v>
+        <v>62</v>
       </c>
       <c r="D18" t="s">
-        <v>40</v>
+        <v>69</v>
       </c>
       <c r="E18" t="s">
-        <v>159</v>
+        <v>222</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>41</v>
+        <v>183</v>
       </c>
       <c r="B19" t="s">
-        <v>6</v>
-      </c>
-      <c r="C19" t="s">
-        <v>11</v>
+        <v>76</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>9</v>
       </c>
       <c r="D19" t="s">
-        <v>42</v>
+        <v>110</v>
       </c>
       <c r="E19" t="s">
-        <v>158</v>
+        <v>143</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>43</v>
+        <v>109</v>
       </c>
       <c r="B20" t="s">
-        <v>6</v>
+        <v>76</v>
       </c>
       <c r="C20" t="s">
-        <v>11</v>
+        <v>62</v>
       </c>
       <c r="D20" t="s">
-        <v>44</v>
+        <v>110</v>
       </c>
       <c r="E20" t="s">
-        <v>157</v>
+        <v>142</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>45</v>
+        <v>184</v>
       </c>
       <c r="B21" t="s">
-        <v>6</v>
-      </c>
-      <c r="C21" t="s">
-        <v>11</v>
+        <v>76</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>9</v>
       </c>
       <c r="D21" t="s">
-        <v>46</v>
+        <v>112</v>
       </c>
       <c r="E21" t="s">
-        <v>156</v>
+        <v>145</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>47</v>
+        <v>111</v>
       </c>
       <c r="B22" t="s">
-        <v>6</v>
+        <v>76</v>
       </c>
       <c r="C22" t="s">
-        <v>11</v>
+        <v>62</v>
       </c>
       <c r="D22" t="s">
-        <v>48</v>
+        <v>112</v>
       </c>
       <c r="E22" t="s">
-        <v>155</v>
+        <v>144</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>49</v>
+        <v>185</v>
       </c>
       <c r="B23" t="s">
-        <v>6</v>
-      </c>
-      <c r="C23" t="s">
-        <v>11</v>
+        <v>76</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>9</v>
       </c>
       <c r="D23" t="s">
-        <v>50</v>
+        <v>114</v>
       </c>
       <c r="E23" t="s">
-        <v>154</v>
+        <v>147</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>51</v>
+        <v>113</v>
       </c>
       <c r="B24" t="s">
-        <v>6</v>
+        <v>76</v>
       </c>
       <c r="C24" t="s">
-        <v>11</v>
+        <v>62</v>
       </c>
       <c r="D24" t="s">
-        <v>52</v>
+        <v>114</v>
       </c>
       <c r="E24" t="s">
-        <v>153</v>
+        <v>146</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>53</v>
+        <v>178</v>
       </c>
       <c r="B25" t="s">
-        <v>6</v>
-      </c>
-      <c r="C25" t="s">
-        <v>11</v>
+        <v>76</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>9</v>
       </c>
       <c r="D25" t="s">
-        <v>54</v>
+        <v>100</v>
       </c>
       <c r="E25" t="s">
-        <v>152</v>
+        <v>133</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>55</v>
+        <v>99</v>
       </c>
       <c r="B26" t="s">
-        <v>6</v>
+        <v>76</v>
       </c>
       <c r="C26" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="D26" t="s">
-        <v>56</v>
+        <v>100</v>
       </c>
       <c r="E26" t="s">
-        <v>151</v>
+        <v>132</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>57</v>
+        <v>86</v>
       </c>
       <c r="B27" t="s">
-        <v>191</v>
+        <v>76</v>
       </c>
       <c r="C27" t="s">
         <v>11</v>
       </c>
       <c r="D27" t="s">
-        <v>59</v>
+        <v>87</v>
       </c>
       <c r="E27" t="s">
-        <v>204</v>
+        <v>124</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>60</v>
+        <v>13</v>
       </c>
       <c r="B28" t="s">
-        <v>191</v>
+        <v>6</v>
       </c>
       <c r="C28" t="s">
         <v>11</v>
       </c>
       <c r="D28" t="s">
-        <v>61</v>
+        <v>14</v>
       </c>
       <c r="E28" t="s">
-        <v>205</v>
+        <v>171</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>197</v>
+        <v>181</v>
       </c>
       <c r="B29" t="s">
-        <v>58</v>
-      </c>
-      <c r="C29" t="s">
-        <v>7</v>
+        <v>76</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>9</v>
       </c>
       <c r="D29" t="s">
-        <v>8</v>
+        <v>106</v>
       </c>
       <c r="E29" t="s">
-        <v>219</v>
+        <v>139</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>198</v>
+        <v>105</v>
       </c>
       <c r="B30" t="s">
-        <v>58</v>
+        <v>76</v>
       </c>
       <c r="C30" t="s">
         <v>7</v>
       </c>
       <c r="D30" t="s">
-        <v>8</v>
+        <v>106</v>
       </c>
       <c r="E30" t="s">
-        <v>206</v>
+        <v>138</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>196</v>
+        <v>182</v>
       </c>
       <c r="B31" t="s">
-        <v>58</v>
-      </c>
-      <c r="C31" t="s">
-        <v>7</v>
+        <v>76</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>9</v>
       </c>
       <c r="D31" t="s">
-        <v>8</v>
-      </c>
-      <c r="E31" s="2" t="s">
-        <v>209</v>
+        <v>108</v>
+      </c>
+      <c r="E31" t="s">
+        <v>141</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>199</v>
+        <v>107</v>
       </c>
       <c r="B32" t="s">
-        <v>58</v>
-      </c>
-      <c r="C32" s="1" t="s">
-        <v>9</v>
+        <v>76</v>
+      </c>
+      <c r="C32" t="s">
+        <v>62</v>
       </c>
       <c r="D32" t="s">
-        <v>8</v>
+        <v>108</v>
       </c>
       <c r="E32" t="s">
-        <v>220</v>
+        <v>140</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>200</v>
+        <v>88</v>
       </c>
       <c r="B33" t="s">
-        <v>58</v>
-      </c>
-      <c r="C33" s="1"/>
+        <v>76</v>
+      </c>
+      <c r="C33" t="s">
+        <v>11</v>
+      </c>
       <c r="D33" t="s">
-        <v>8</v>
+        <v>89</v>
       </c>
       <c r="E33" t="s">
-        <v>207</v>
+        <v>125</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>201</v>
+        <v>90</v>
       </c>
       <c r="B34" t="s">
-        <v>58</v>
-      </c>
-      <c r="C34" s="1"/>
+        <v>76</v>
+      </c>
+      <c r="C34" t="s">
+        <v>11</v>
+      </c>
       <c r="D34" t="s">
-        <v>8</v>
+        <v>91</v>
       </c>
       <c r="E34" t="s">
-        <v>210</v>
+        <v>126</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>193</v>
-      </c>
-      <c r="B35" s="2" t="s">
-        <v>191</v>
+        <v>84</v>
+      </c>
+      <c r="B35" t="s">
+        <v>76</v>
       </c>
       <c r="C35" t="s">
-        <v>62</v>
+        <v>11</v>
       </c>
       <c r="D35" t="s">
-        <v>63</v>
+        <v>85</v>
       </c>
       <c r="E35" t="s">
-        <v>211</v>
+        <v>123</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>202</v>
-      </c>
-      <c r="B36" s="2" t="s">
-        <v>191</v>
-      </c>
-      <c r="C36" s="1" t="s">
-        <v>9</v>
+        <v>75</v>
+      </c>
+      <c r="B36" t="s">
+        <v>76</v>
+      </c>
+      <c r="C36" t="s">
+        <v>7</v>
       </c>
       <c r="D36" t="s">
-        <v>63</v>
+        <v>77</v>
       </c>
       <c r="E36" t="s">
-        <v>208</v>
+        <v>119</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
+        <v>57</v>
+      </c>
+      <c r="B37" t="s">
+        <v>190</v>
+      </c>
+      <c r="C37" t="s">
+        <v>11</v>
+      </c>
+      <c r="D37" t="s">
+        <v>59</v>
+      </c>
+      <c r="E37" t="s">
         <v>203</v>
-      </c>
-      <c r="B37" s="2" t="s">
-        <v>191</v>
-      </c>
-      <c r="C37" s="1"/>
-      <c r="D37" t="s">
-        <v>63</v>
-      </c>
-      <c r="E37" t="s">
-        <v>212</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>64</v>
-      </c>
-      <c r="B38" s="2" t="s">
-        <v>191</v>
+        <v>37</v>
+      </c>
+      <c r="B38" t="s">
+        <v>6</v>
       </c>
       <c r="C38" t="s">
-        <v>62</v>
+        <v>11</v>
       </c>
       <c r="D38" t="s">
-        <v>65</v>
+        <v>38</v>
       </c>
       <c r="E38" t="s">
-        <v>213</v>
+        <v>159</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>188</v>
-      </c>
-      <c r="B39" s="2" t="s">
-        <v>191</v>
-      </c>
-      <c r="C39" s="1" t="s">
-        <v>9</v>
+        <v>39</v>
+      </c>
+      <c r="B39" t="s">
+        <v>6</v>
+      </c>
+      <c r="C39" t="s">
+        <v>11</v>
       </c>
       <c r="D39" t="s">
-        <v>65</v>
+        <v>40</v>
       </c>
       <c r="E39" t="s">
-        <v>214</v>
+        <v>158</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>66</v>
-      </c>
-      <c r="B40" s="2" t="s">
-        <v>191</v>
+        <v>41</v>
+      </c>
+      <c r="B40" t="s">
+        <v>6</v>
       </c>
       <c r="C40" t="s">
-        <v>62</v>
+        <v>11</v>
       </c>
       <c r="D40" t="s">
-        <v>67</v>
+        <v>42</v>
       </c>
       <c r="E40" t="s">
-        <v>221</v>
+        <v>157</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>189</v>
-      </c>
-      <c r="B41" s="2" t="s">
-        <v>191</v>
-      </c>
-      <c r="C41" s="1" t="s">
-        <v>9</v>
+        <v>43</v>
+      </c>
+      <c r="B41" t="s">
+        <v>6</v>
+      </c>
+      <c r="C41" t="s">
+        <v>11</v>
       </c>
       <c r="D41" t="s">
-        <v>67</v>
+        <v>44</v>
       </c>
       <c r="E41" t="s">
-        <v>222</v>
+        <v>156</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>68</v>
-      </c>
-      <c r="B42" s="2" t="s">
-        <v>191</v>
+        <v>45</v>
+      </c>
+      <c r="B42" t="s">
+        <v>6</v>
       </c>
       <c r="C42" t="s">
-        <v>62</v>
+        <v>11</v>
       </c>
       <c r="D42" t="s">
-        <v>69</v>
+        <v>46</v>
       </c>
       <c r="E42" t="s">
-        <v>223</v>
+        <v>155</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
+        <v>187</v>
+      </c>
+      <c r="B43" s="2" t="s">
         <v>190</v>
-      </c>
-      <c r="B43" s="2" t="s">
-        <v>191</v>
       </c>
       <c r="C43" s="1" t="s">
         <v>9</v>
       </c>
       <c r="D43" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="E43" t="s">
-        <v>224</v>
+        <v>213</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>70</v>
-      </c>
-      <c r="B44" t="s">
-        <v>58</v>
+        <v>64</v>
+      </c>
+      <c r="B44" s="2" t="s">
+        <v>190</v>
       </c>
       <c r="C44" t="s">
         <v>62</v>
       </c>
       <c r="D44" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="E44" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B45" t="s">
         <v>58</v>
@@ -1828,605 +1834,604 @@
         <v>71</v>
       </c>
       <c r="E45" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B46" t="s">
         <v>58</v>
       </c>
       <c r="C46" t="s">
-        <v>11</v>
+        <v>62</v>
       </c>
       <c r="D46" t="s">
-        <v>12</v>
+        <v>71</v>
       </c>
       <c r="E46" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>73</v>
+        <v>186</v>
       </c>
       <c r="B47" t="s">
-        <v>58</v>
-      </c>
-      <c r="C47" t="s">
-        <v>11</v>
+        <v>6</v>
+      </c>
+      <c r="C47" s="1" t="s">
+        <v>9</v>
       </c>
       <c r="D47" t="s">
-        <v>74</v>
+        <v>8</v>
       </c>
       <c r="E47" t="s">
-        <v>218</v>
+        <v>173</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>76</v>
+        <v>198</v>
       </c>
       <c r="B48" t="s">
-        <v>77</v>
-      </c>
-      <c r="C48" t="s">
-        <v>7</v>
+        <v>58</v>
+      </c>
+      <c r="C48" s="1" t="s">
+        <v>9</v>
       </c>
       <c r="D48" t="s">
-        <v>78</v>
+        <v>8</v>
       </c>
       <c r="E48" t="s">
-        <v>120</v>
+        <v>219</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>79</v>
+        <v>176</v>
       </c>
       <c r="B49" t="s">
-        <v>77</v>
-      </c>
-      <c r="C49" t="s">
-        <v>11</v>
+        <v>191</v>
+      </c>
+      <c r="C49" s="1" t="s">
+        <v>9</v>
       </c>
       <c r="D49" t="s">
-        <v>80</v>
+        <v>8</v>
       </c>
       <c r="E49" t="s">
-        <v>121</v>
+        <v>194</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>81</v>
+        <v>5</v>
       </c>
       <c r="B50" t="s">
-        <v>77</v>
+        <v>6</v>
       </c>
       <c r="C50" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="D50" t="s">
-        <v>82</v>
+        <v>8</v>
       </c>
       <c r="E50" t="s">
-        <v>122</v>
+        <v>174</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>83</v>
+        <v>196</v>
       </c>
       <c r="B51" t="s">
-        <v>77</v>
+        <v>58</v>
       </c>
       <c r="C51" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="D51" t="s">
-        <v>84</v>
+        <v>8</v>
       </c>
       <c r="E51" t="s">
-        <v>123</v>
+        <v>218</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>85</v>
+        <v>197</v>
       </c>
       <c r="B52" t="s">
-        <v>77</v>
+        <v>58</v>
       </c>
       <c r="C52" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="D52" t="s">
-        <v>86</v>
+        <v>8</v>
       </c>
       <c r="E52" t="s">
-        <v>124</v>
+        <v>205</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>87</v>
+        <v>195</v>
       </c>
       <c r="B53" t="s">
-        <v>77</v>
+        <v>58</v>
       </c>
       <c r="C53" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="D53" t="s">
-        <v>88</v>
-      </c>
-      <c r="E53" t="s">
-        <v>125</v>
+        <v>8</v>
+      </c>
+      <c r="E53" s="2" t="s">
+        <v>208</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>89</v>
+        <v>74</v>
       </c>
       <c r="B54" t="s">
-        <v>77</v>
+        <v>191</v>
       </c>
       <c r="C54" t="s">
-        <v>11</v>
+        <v>62</v>
       </c>
       <c r="D54" t="s">
-        <v>90</v>
+        <v>8</v>
       </c>
       <c r="E54" t="s">
-        <v>126</v>
+        <v>193</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>91</v>
+        <v>199</v>
       </c>
       <c r="B55" t="s">
-        <v>77</v>
-      </c>
-      <c r="C55" t="s">
-        <v>11</v>
-      </c>
+        <v>58</v>
+      </c>
+      <c r="C55" s="1"/>
       <c r="D55" t="s">
-        <v>92</v>
+        <v>8</v>
       </c>
       <c r="E55" t="s">
-        <v>127</v>
+        <v>206</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>93</v>
+        <v>200</v>
       </c>
       <c r="B56" t="s">
-        <v>77</v>
-      </c>
-      <c r="C56" t="s">
-        <v>7</v>
-      </c>
+        <v>58</v>
+      </c>
+      <c r="C56" s="1"/>
       <c r="D56" t="s">
-        <v>94</v>
+        <v>8</v>
       </c>
       <c r="E56" t="s">
-        <v>128</v>
+        <v>209</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>95</v>
+        <v>15</v>
       </c>
       <c r="B57" t="s">
-        <v>77</v>
+        <v>6</v>
       </c>
       <c r="C57" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="D57" t="s">
-        <v>96</v>
+        <v>16</v>
       </c>
       <c r="E57" t="s">
-        <v>129</v>
+        <v>170</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>97</v>
+        <v>115</v>
       </c>
       <c r="B58" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C58" t="s">
         <v>11</v>
       </c>
       <c r="D58" t="s">
-        <v>98</v>
+        <v>116</v>
       </c>
       <c r="E58" t="s">
-        <v>130</v>
+        <v>148</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>99</v>
+        <v>47</v>
       </c>
       <c r="B59" t="s">
-        <v>77</v>
+        <v>6</v>
       </c>
       <c r="C59" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="D59" t="s">
-        <v>63</v>
+        <v>48</v>
       </c>
       <c r="E59" t="s">
-        <v>131</v>
+        <v>154</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>178</v>
+        <v>49</v>
       </c>
       <c r="B60" t="s">
-        <v>77</v>
-      </c>
-      <c r="C60" s="1" t="s">
-        <v>9</v>
+        <v>6</v>
+      </c>
+      <c r="C60" t="s">
+        <v>11</v>
       </c>
       <c r="D60" t="s">
-        <v>63</v>
+        <v>50</v>
       </c>
       <c r="E60" t="s">
-        <v>132</v>
+        <v>153</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>100</v>
+        <v>51</v>
       </c>
       <c r="B61" t="s">
-        <v>77</v>
+        <v>6</v>
       </c>
       <c r="C61" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="D61" t="s">
-        <v>101</v>
+        <v>52</v>
       </c>
       <c r="E61" t="s">
-        <v>133</v>
+        <v>152</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>179</v>
+        <v>53</v>
       </c>
       <c r="B62" t="s">
-        <v>77</v>
-      </c>
-      <c r="C62" s="1" t="s">
-        <v>9</v>
+        <v>6</v>
+      </c>
+      <c r="C62" t="s">
+        <v>11</v>
       </c>
       <c r="D62" t="s">
-        <v>101</v>
+        <v>54</v>
       </c>
       <c r="E62" t="s">
-        <v>134</v>
+        <v>151</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>102</v>
+        <v>55</v>
       </c>
       <c r="B63" t="s">
-        <v>77</v>
+        <v>6</v>
       </c>
       <c r="C63" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="D63" t="s">
-        <v>103</v>
+        <v>56</v>
       </c>
       <c r="E63" t="s">
-        <v>135</v>
+        <v>150</v>
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>180</v>
+        <v>117</v>
       </c>
       <c r="B64" t="s">
-        <v>77</v>
-      </c>
-      <c r="C64" s="1" t="s">
-        <v>9</v>
+        <v>76</v>
+      </c>
+      <c r="C64" t="s">
+        <v>11</v>
       </c>
       <c r="D64" t="s">
-        <v>103</v>
+        <v>118</v>
       </c>
       <c r="E64" t="s">
-        <v>136</v>
+        <v>149</v>
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>104</v>
+        <v>10</v>
       </c>
       <c r="B65" t="s">
-        <v>77</v>
+        <v>6</v>
       </c>
       <c r="C65" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="D65" t="s">
-        <v>105</v>
+        <v>12</v>
       </c>
       <c r="E65" t="s">
-        <v>137</v>
+        <v>172</v>
       </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>181</v>
+        <v>72</v>
       </c>
       <c r="B66" t="s">
-        <v>77</v>
-      </c>
-      <c r="C66" s="1" t="s">
-        <v>9</v>
+        <v>58</v>
+      </c>
+      <c r="C66" t="s">
+        <v>11</v>
       </c>
       <c r="D66" t="s">
-        <v>105</v>
+        <v>12</v>
       </c>
       <c r="E66" t="s">
-        <v>138</v>
+        <v>216</v>
       </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>106</v>
+        <v>78</v>
       </c>
       <c r="B67" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C67" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="D67" t="s">
-        <v>107</v>
+        <v>79</v>
       </c>
       <c r="E67" t="s">
-        <v>139</v>
+        <v>120</v>
       </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>182</v>
-      </c>
-      <c r="B68" t="s">
-        <v>77</v>
+        <v>188</v>
+      </c>
+      <c r="B68" s="2" t="s">
+        <v>190</v>
       </c>
       <c r="C68" s="1" t="s">
         <v>9</v>
       </c>
       <c r="D68" t="s">
-        <v>107</v>
+        <v>67</v>
       </c>
       <c r="E68" t="s">
-        <v>140</v>
+        <v>221</v>
       </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>108</v>
-      </c>
-      <c r="B69" t="s">
-        <v>77</v>
+        <v>66</v>
+      </c>
+      <c r="B69" s="2" t="s">
+        <v>190</v>
       </c>
       <c r="C69" t="s">
         <v>62</v>
       </c>
       <c r="D69" t="s">
-        <v>109</v>
+        <v>67</v>
       </c>
       <c r="E69" t="s">
-        <v>141</v>
+        <v>220</v>
       </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>183</v>
-      </c>
-      <c r="B70" t="s">
-        <v>77</v>
+        <v>201</v>
+      </c>
+      <c r="B70" s="2" t="s">
+        <v>190</v>
       </c>
       <c r="C70" s="1" t="s">
         <v>9</v>
       </c>
       <c r="D70" t="s">
-        <v>109</v>
+        <v>63</v>
       </c>
       <c r="E70" t="s">
-        <v>142</v>
+        <v>207</v>
       </c>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>110</v>
+        <v>177</v>
       </c>
       <c r="B71" t="s">
-        <v>77</v>
-      </c>
-      <c r="C71" t="s">
-        <v>62</v>
+        <v>76</v>
+      </c>
+      <c r="C71" s="1" t="s">
+        <v>9</v>
       </c>
       <c r="D71" t="s">
-        <v>111</v>
+        <v>63</v>
       </c>
       <c r="E71" t="s">
-        <v>143</v>
+        <v>131</v>
       </c>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
-        <v>184</v>
-      </c>
-      <c r="B72" t="s">
-        <v>77</v>
-      </c>
-      <c r="C72" s="1" t="s">
-        <v>9</v>
+        <v>192</v>
+      </c>
+      <c r="B72" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="C72" t="s">
+        <v>62</v>
       </c>
       <c r="D72" t="s">
-        <v>111</v>
+        <v>63</v>
       </c>
       <c r="E72" t="s">
-        <v>144</v>
+        <v>210</v>
       </c>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
-        <v>112</v>
+        <v>98</v>
       </c>
       <c r="B73" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C73" t="s">
-        <v>62</v>
+        <v>7</v>
       </c>
       <c r="D73" t="s">
-        <v>113</v>
+        <v>63</v>
       </c>
       <c r="E73" t="s">
-        <v>145</v>
+        <v>130</v>
       </c>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
-        <v>185</v>
-      </c>
-      <c r="B74" t="s">
-        <v>77</v>
-      </c>
-      <c r="C74" s="1" t="s">
-        <v>9</v>
-      </c>
+        <v>202</v>
+      </c>
+      <c r="B74" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="C74" s="1"/>
       <c r="D74" t="s">
-        <v>113</v>
+        <v>63</v>
       </c>
       <c r="E74" t="s">
-        <v>146</v>
+        <v>211</v>
       </c>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
-        <v>114</v>
+        <v>82</v>
       </c>
       <c r="B75" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C75" t="s">
-        <v>62</v>
+        <v>11</v>
       </c>
       <c r="D75" t="s">
-        <v>115</v>
+        <v>83</v>
       </c>
       <c r="E75" t="s">
-        <v>147</v>
+        <v>122</v>
       </c>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
-        <v>186</v>
+        <v>179</v>
       </c>
       <c r="B76" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C76" s="1" t="s">
         <v>9</v>
       </c>
       <c r="D76" t="s">
-        <v>115</v>
+        <v>102</v>
       </c>
       <c r="E76" t="s">
-        <v>148</v>
+        <v>135</v>
       </c>
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
-        <v>116</v>
+        <v>101</v>
       </c>
       <c r="B77" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C77" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="D77" t="s">
-        <v>117</v>
+        <v>102</v>
       </c>
       <c r="E77" t="s">
-        <v>149</v>
+        <v>134</v>
       </c>
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
-        <v>118</v>
+        <v>94</v>
       </c>
       <c r="B78" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C78" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="D78" t="s">
-        <v>119</v>
+        <v>95</v>
       </c>
       <c r="E78" t="s">
-        <v>150</v>
+        <v>128</v>
       </c>
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
-        <v>75</v>
+        <v>180</v>
       </c>
       <c r="B79" t="s">
-        <v>192</v>
-      </c>
-      <c r="C79" t="s">
-        <v>62</v>
+        <v>76</v>
+      </c>
+      <c r="C79" s="1" t="s">
+        <v>9</v>
       </c>
       <c r="D79" t="s">
-        <v>8</v>
+        <v>104</v>
       </c>
       <c r="E79" t="s">
-        <v>194</v>
+        <v>137</v>
       </c>
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
-        <v>177</v>
+        <v>103</v>
       </c>
       <c r="B80" t="s">
-        <v>192</v>
-      </c>
-      <c r="C80" s="1" t="s">
-        <v>9</v>
+        <v>76</v>
+      </c>
+      <c r="C80" t="s">
+        <v>7</v>
       </c>
       <c r="D80" t="s">
-        <v>8</v>
+        <v>104</v>
       </c>
       <c r="E80" t="s">
-        <v>195</v>
+        <v>136</v>
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:E80">
+    <sortState ref="A2:E80">
+      <sortCondition ref="D1:D80"/>
+    </sortState>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
clean up script folder
</commit_message>
<xml_diff>
--- a/etl/source/metadata.xlsx
+++ b/etl/source/metadata.xlsx
@@ -683,9 +683,6 @@
     <t>ddf--datapoints--SexRatio_MalePer100Female--by--ref_area_code--year--variant--agebroad</t>
   </si>
   <si>
-    <t>ddf--datapoints--FeminityRato_FemalePer100Male--by--ref_area_code--year--variant--agebroad</t>
-  </si>
-  <si>
     <t>ddf--datapoints--Population--by--ref_area_code--year--variant--age1yearinterval</t>
   </si>
   <si>
@@ -705,6 +702,9 @@
   </si>
   <si>
     <t>FeminityRatio_FemalePer100Male</t>
+  </si>
+  <si>
+    <t>ddf--datapoints--FeminityRatio_FemalePer100Male--by--ref_area_code--year--variant--agebroad</t>
   </si>
 </sst>
 </file>
@@ -1060,8 +1060,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E80"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1304,10 +1304,10 @@
         <v>11</v>
       </c>
       <c r="D14" t="s">
+        <v>223</v>
+      </c>
+      <c r="E14" t="s">
         <v>224</v>
-      </c>
-      <c r="E14" t="s">
-        <v>217</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
@@ -1358,7 +1358,7 @@
         <v>69</v>
       </c>
       <c r="E17" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.2">
@@ -1375,7 +1375,7 @@
         <v>69</v>
       </c>
       <c r="E18" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.2">
@@ -1885,7 +1885,7 @@
         <v>8</v>
       </c>
       <c r="E48" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.2">
@@ -1936,7 +1936,7 @@
         <v>8</v>
       </c>
       <c r="E51" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.2">
@@ -2221,7 +2221,7 @@
         <v>67</v>
       </c>
       <c r="E68" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.2">
@@ -2238,7 +2238,7 @@
         <v>67</v>
       </c>
       <c r="E69" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
includes Demography Interpolated file AND variants are not seperated by underscore char
</commit_message>
<xml_diff>
--- a/etl/source/metadata.xlsx
+++ b/etl/source/metadata.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="9600" yWindow="3760" windowWidth="28800" windowHeight="16240" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="38400" windowHeight="19540" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="metadata" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="397" uniqueCount="225">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="403" uniqueCount="229">
   <si>
     <t>FileName</t>
   </si>
@@ -705,6 +705,18 @@
   </si>
   <si>
     <t>ddf--datapoints--Under60MortalityPer1000livebirth--by--ref_area_code--year--variant--freq</t>
+  </si>
+  <si>
+    <t>Include</t>
+  </si>
+  <si>
+    <t>NewFormat</t>
+  </si>
+  <si>
+    <t>ddf--datapoints--NewFormat--by--ref_area_code--year--variant-</t>
+  </si>
+  <si>
+    <t>WPP2015_INT_F01_ANNUAL_DEMOGRAPHIC_INDICATORS.XLS</t>
   </si>
 </sst>
 </file>
@@ -1058,10 +1070,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E80"/>
+  <dimension ref="A1:F81"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:E80"/>
+    <sheetView tabSelected="1" topLeftCell="A47" workbookViewId="0">
+      <selection activeCell="E75" sqref="E75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1072,7 +1084,7 @@
     <col min="5" max="5" width="83" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1088,8 +1100,11 @@
       <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F1" s="1" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>5</v>
       </c>
@@ -1105,8 +1120,11 @@
       <c r="E2" s="1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>10</v>
       </c>
@@ -1122,8 +1140,11 @@
       <c r="E3" s="1" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>14</v>
       </c>
@@ -1139,8 +1160,11 @@
       <c r="E4" s="1" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>17</v>
       </c>
@@ -1156,8 +1180,11 @@
       <c r="E5" s="1" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>20</v>
       </c>
@@ -1173,8 +1200,11 @@
       <c r="E6" s="1" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>23</v>
       </c>
@@ -1190,8 +1220,11 @@
       <c r="E7" s="1" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>26</v>
       </c>
@@ -1207,8 +1240,11 @@
       <c r="E8" s="1" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>29</v>
       </c>
@@ -1224,8 +1260,11 @@
       <c r="E9" s="1" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>32</v>
       </c>
@@ -1241,8 +1280,11 @@
       <c r="E10" s="1" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>35</v>
       </c>
@@ -1258,8 +1300,11 @@
       <c r="E11" s="1" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>38</v>
       </c>
@@ -1275,8 +1320,11 @@
       <c r="E12" s="1" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>41</v>
       </c>
@@ -1292,8 +1340,11 @@
       <c r="E13" s="1" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>44</v>
       </c>
@@ -1309,8 +1360,11 @@
       <c r="E14" s="1" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>48</v>
       </c>
@@ -1326,8 +1380,11 @@
       <c r="E15" s="1" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>52</v>
       </c>
@@ -1343,8 +1400,11 @@
       <c r="E16" s="1" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
         <v>56</v>
       </c>
@@ -1360,8 +1420,11 @@
       <c r="E17" s="1" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
         <v>60</v>
       </c>
@@ -1377,8 +1440,11 @@
       <c r="E18" s="1" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
         <v>63</v>
       </c>
@@ -1394,8 +1460,11 @@
       <c r="E19" s="1" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
         <v>66</v>
       </c>
@@ -1411,8 +1480,11 @@
       <c r="E20" s="1" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
         <v>68</v>
       </c>
@@ -1428,8 +1500,11 @@
       <c r="E21" s="1" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
         <v>71</v>
       </c>
@@ -1445,8 +1520,11 @@
       <c r="E22" s="1" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
         <v>73</v>
       </c>
@@ -1462,8 +1540,11 @@
       <c r="E23" s="1" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
         <v>76</v>
       </c>
@@ -1479,8 +1560,11 @@
       <c r="E24" s="1" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
         <v>78</v>
       </c>
@@ -1496,8 +1580,11 @@
       <c r="E25" s="1" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
         <v>81</v>
       </c>
@@ -1513,8 +1600,11 @@
       <c r="E26" s="1" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F26">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
         <v>83</v>
       </c>
@@ -1530,8 +1620,11 @@
       <c r="E27" s="1" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F27">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
         <v>86</v>
       </c>
@@ -1547,8 +1640,11 @@
       <c r="E28" s="1" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F28">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
         <v>89</v>
       </c>
@@ -1564,8 +1660,11 @@
       <c r="E29" s="1" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F29">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
         <v>92</v>
       </c>
@@ -1581,8 +1680,11 @@
       <c r="E30" s="1" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F30">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
         <v>94</v>
       </c>
@@ -1598,8 +1700,11 @@
       <c r="E31" s="1" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F31">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
         <v>97</v>
       </c>
@@ -1615,8 +1720,11 @@
       <c r="E32" s="1" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F32">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
         <v>99</v>
       </c>
@@ -1632,8 +1740,11 @@
       <c r="E33" s="1" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F33">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
         <v>102</v>
       </c>
@@ -1649,8 +1760,11 @@
       <c r="E34" s="1" t="s">
         <v>104</v>
       </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
         <v>105</v>
       </c>
@@ -1666,8 +1780,11 @@
       <c r="E35" s="1" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A36" s="1" t="s">
         <v>108</v>
       </c>
@@ -1683,8 +1800,11 @@
       <c r="E36" s="1" t="s">
         <v>110</v>
       </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F36">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
         <v>111</v>
       </c>
@@ -1700,8 +1820,11 @@
       <c r="E37" s="1" t="s">
         <v>113</v>
       </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F37">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A38" s="1" t="s">
         <v>114</v>
       </c>
@@ -1717,8 +1840,11 @@
       <c r="E38" s="1" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F38">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A39" s="1" t="s">
         <v>117</v>
       </c>
@@ -1734,8 +1860,11 @@
       <c r="E39" s="1" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F39">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A40" s="1" t="s">
         <v>120</v>
       </c>
@@ -1751,8 +1880,11 @@
       <c r="E40" s="1" t="s">
         <v>122</v>
       </c>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F40">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A41" s="1" t="s">
         <v>123</v>
       </c>
@@ -1768,8 +1900,11 @@
       <c r="E41" s="1" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F41">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A42" s="1" t="s">
         <v>126</v>
       </c>
@@ -1785,8 +1920,11 @@
       <c r="E42" s="1" t="s">
         <v>128</v>
       </c>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F42">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A43" s="1" t="s">
         <v>129</v>
       </c>
@@ -1802,8 +1940,11 @@
       <c r="E43" s="1" t="s">
         <v>131</v>
       </c>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F43">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A44" s="1" t="s">
         <v>132</v>
       </c>
@@ -1819,8 +1960,11 @@
       <c r="E44" s="1" t="s">
         <v>133</v>
       </c>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F44">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A45" s="1" t="s">
         <v>134</v>
       </c>
@@ -1836,8 +1980,11 @@
       <c r="E45" s="1" t="s">
         <v>136</v>
       </c>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F45">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A46" s="1" t="s">
         <v>137</v>
       </c>
@@ -1853,8 +2000,11 @@
       <c r="E46" s="1" t="s">
         <v>138</v>
       </c>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F46">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A47" s="1" t="s">
         <v>139</v>
       </c>
@@ -1870,8 +2020,11 @@
       <c r="E47" s="1" t="s">
         <v>141</v>
       </c>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F47">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A48" s="1" t="s">
         <v>142</v>
       </c>
@@ -1887,8 +2040,11 @@
       <c r="E48" s="1" t="s">
         <v>143</v>
       </c>
-    </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F48">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A49" s="1" t="s">
         <v>144</v>
       </c>
@@ -1904,8 +2060,11 @@
       <c r="E49" s="1" t="s">
         <v>146</v>
       </c>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F49">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A50" s="1" t="s">
         <v>147</v>
       </c>
@@ -1921,8 +2080,11 @@
       <c r="E50" s="1" t="s">
         <v>148</v>
       </c>
-    </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F50">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A51" s="1" t="s">
         <v>149</v>
       </c>
@@ -1938,8 +2100,11 @@
       <c r="E51" s="1" t="s">
         <v>150</v>
       </c>
-    </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F51">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A52" s="1" t="s">
         <v>151</v>
       </c>
@@ -1955,8 +2120,11 @@
       <c r="E52" s="1" t="s">
         <v>152</v>
       </c>
-    </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F52">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A53" s="1" t="s">
         <v>153</v>
       </c>
@@ -1972,8 +2140,11 @@
       <c r="E53" s="1" t="s">
         <v>154</v>
       </c>
-    </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F53">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A54" s="1" t="s">
         <v>155</v>
       </c>
@@ -1989,8 +2160,11 @@
       <c r="E54" s="1" t="s">
         <v>156</v>
       </c>
-    </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F54">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A55" s="1" t="s">
         <v>157</v>
       </c>
@@ -2004,8 +2178,11 @@
       <c r="E55" s="1" t="s">
         <v>158</v>
       </c>
-    </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F55">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A56" s="1" t="s">
         <v>159</v>
       </c>
@@ -2019,8 +2196,11 @@
       <c r="E56" s="1" t="s">
         <v>160</v>
       </c>
-    </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F56">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A57" s="1" t="s">
         <v>161</v>
       </c>
@@ -2036,8 +2216,11 @@
       <c r="E57" s="1" t="s">
         <v>163</v>
       </c>
-    </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F57">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A58" s="1" t="s">
         <v>164</v>
       </c>
@@ -2053,8 +2236,11 @@
       <c r="E58" s="1" t="s">
         <v>166</v>
       </c>
-    </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F58">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A59" s="1" t="s">
         <v>167</v>
       </c>
@@ -2070,8 +2256,11 @@
       <c r="E59" s="1" t="s">
         <v>169</v>
       </c>
-    </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F59">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A60" s="1" t="s">
         <v>170</v>
       </c>
@@ -2087,8 +2276,11 @@
       <c r="E60" s="1" t="s">
         <v>172</v>
       </c>
-    </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F60">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A61" s="1" t="s">
         <v>173</v>
       </c>
@@ -2104,8 +2296,11 @@
       <c r="E61" s="1" t="s">
         <v>175</v>
       </c>
-    </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F61">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A62" s="1" t="s">
         <v>176</v>
       </c>
@@ -2121,8 +2316,11 @@
       <c r="E62" s="1" t="s">
         <v>178</v>
       </c>
-    </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F62">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A63" s="1" t="s">
         <v>179</v>
       </c>
@@ -2138,8 +2336,11 @@
       <c r="E63" s="1" t="s">
         <v>181</v>
       </c>
-    </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F63">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A64" s="1" t="s">
         <v>182</v>
       </c>
@@ -2155,8 +2356,11 @@
       <c r="E64" s="1" t="s">
         <v>184</v>
       </c>
-    </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F64">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A65" s="1" t="s">
         <v>185</v>
       </c>
@@ -2172,8 +2376,11 @@
       <c r="E65" s="1" t="s">
         <v>187</v>
       </c>
-    </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F65">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A66" s="1" t="s">
         <v>188</v>
       </c>
@@ -2189,8 +2396,11 @@
       <c r="E66" s="1" t="s">
         <v>189</v>
       </c>
-    </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F66">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A67" s="1" t="s">
         <v>190</v>
       </c>
@@ -2206,8 +2416,11 @@
       <c r="E67" s="1" t="s">
         <v>192</v>
       </c>
-    </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F67">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A68" s="1" t="s">
         <v>193</v>
       </c>
@@ -2223,8 +2436,11 @@
       <c r="E68" s="1" t="s">
         <v>195</v>
       </c>
-    </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F68">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A69" s="1" t="s">
         <v>196</v>
       </c>
@@ -2240,8 +2456,11 @@
       <c r="E69" s="1" t="s">
         <v>197</v>
       </c>
-    </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F69">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A70" s="1" t="s">
         <v>198</v>
       </c>
@@ -2257,8 +2476,11 @@
       <c r="E70" s="1" t="s">
         <v>200</v>
       </c>
-    </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F70">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A71" s="1" t="s">
         <v>201</v>
       </c>
@@ -2274,8 +2496,11 @@
       <c r="E71" s="1" t="s">
         <v>202</v>
       </c>
-    </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F71">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A72" s="1" t="s">
         <v>203</v>
       </c>
@@ -2291,8 +2516,11 @@
       <c r="E72" s="1" t="s">
         <v>204</v>
       </c>
-    </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F72">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A73" s="1" t="s">
         <v>205</v>
       </c>
@@ -2308,8 +2536,11 @@
       <c r="E73" s="1" t="s">
         <v>206</v>
       </c>
-    </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F73">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A74" s="1" t="s">
         <v>207</v>
       </c>
@@ -2323,8 +2554,11 @@
       <c r="E74" s="1" t="s">
         <v>208</v>
       </c>
-    </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F74">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A75" s="1" t="s">
         <v>209</v>
       </c>
@@ -2340,8 +2574,11 @@
       <c r="E75" s="1" t="s">
         <v>211</v>
       </c>
-    </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F75">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A76" s="1" t="s">
         <v>212</v>
       </c>
@@ -2357,8 +2594,11 @@
       <c r="E76" s="1" t="s">
         <v>214</v>
       </c>
-    </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F76">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="77" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A77" s="1" t="s">
         <v>215</v>
       </c>
@@ -2374,8 +2614,11 @@
       <c r="E77" s="1" t="s">
         <v>216</v>
       </c>
-    </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F77">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="78" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A78" s="1" t="s">
         <v>217</v>
       </c>
@@ -2391,8 +2634,11 @@
       <c r="E78" s="1" t="s">
         <v>219</v>
       </c>
-    </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F78">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="79" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A79" s="1" t="s">
         <v>220</v>
       </c>
@@ -2408,8 +2654,11 @@
       <c r="E79" s="1" t="s">
         <v>222</v>
       </c>
-    </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F79">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="80" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A80" s="1" t="s">
         <v>223</v>
       </c>
@@ -2424,6 +2673,29 @@
       </c>
       <c r="E80" s="1" t="s">
         <v>224</v>
+      </c>
+      <c r="F80">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="81" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A81" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="B81" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="C81" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D81" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="E81" t="s">
+        <v>227</v>
+      </c>
+      <c r="F81">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Include rest of the interpolated data
</commit_message>
<xml_diff>
--- a/etl/source/metadata.xlsx
+++ b/etl/source/metadata.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/Data/GapMinder/ddf--unpop--wpp_population/etl/source/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/Data/GapMinder/testWorkDir/etl/source/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -13,9 +13,12 @@
   </bookViews>
   <sheets>
     <sheet name="metadata" sheetId="1" r:id="rId1"/>
+    <sheet name="DemographyFormat" sheetId="2" r:id="rId2"/>
+    <sheet name="BroadAgeMap" sheetId="3" r:id="rId3"/>
+    <sheet name="DependencyFormat" sheetId="4" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">metadata!$A$1:$E$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">metadata!$A$1:$G$87</definedName>
   </definedNames>
   <calcPr calcId="0" concurrentCalc="0"/>
   <extLst>
@@ -30,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="403" uniqueCount="229">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="672" uniqueCount="408">
   <si>
     <t>FileName</t>
   </si>
@@ -713,10 +716,547 @@
     <t>NewFormat</t>
   </si>
   <si>
-    <t>ddf--datapoints--NewFormat--by--ref_area_code--year--variant-</t>
-  </si>
-  <si>
     <t>WPP2015_INT_F01_ANNUAL_DEMOGRAPHIC_INDICATORS.XLS</t>
+  </si>
+  <si>
+    <t>IndicatorInitial</t>
+  </si>
+  <si>
+    <t>IndicatorDest</t>
+  </si>
+  <si>
+    <t>DestFolder</t>
+  </si>
+  <si>
+    <t>Deaths (thousands)</t>
+  </si>
+  <si>
+    <t>ddf--datapoints--NewFormat--by--ref_area_code--year--variant</t>
+  </si>
+  <si>
+    <t>Male deaths (thousands);Female deaths (thousands)</t>
+  </si>
+  <si>
+    <t>ddf--datapoints--NewFormat--by--ref_area_code--year--variant--gender</t>
+  </si>
+  <si>
+    <t>Crude death rate (deaths per 1,000 population)</t>
+  </si>
+  <si>
+    <t>crudedeathrateper1000population</t>
+  </si>
+  <si>
+    <t>Life expectancy at birth, both sexes combined (years)</t>
+  </si>
+  <si>
+    <t>Life expectancy at birth, males (years);Life expectancy at birth, females (years)</t>
+  </si>
+  <si>
+    <t>Infant deaths, both sexes combined (under age 1, thousands)</t>
+  </si>
+  <si>
+    <t>InfantMortality</t>
+  </si>
+  <si>
+    <t>Infant mortality rate (infant deaths per 1,000 live births)</t>
+  </si>
+  <si>
+    <t>Total survivors to age 1 (thousands)</t>
+  </si>
+  <si>
+    <t>totalsurvivors_under_one_yearage</t>
+  </si>
+  <si>
+    <t>Under-five mortality (deaths under age 5 per 1,000 live births)</t>
+  </si>
+  <si>
+    <t>under_five_mortality</t>
+  </si>
+  <si>
+    <t>Births (thousands)</t>
+  </si>
+  <si>
+    <t>noofbirth</t>
+  </si>
+  <si>
+    <t>Crude birth rate (births per 1,000 population)</t>
+  </si>
+  <si>
+    <t>birthper1000population</t>
+  </si>
+  <si>
+    <t>Total fertility (children per woman)</t>
+  </si>
+  <si>
+    <t>Total population natural change / increase (thousands)</t>
+  </si>
+  <si>
+    <t>PopulationNaturalChange</t>
+  </si>
+  <si>
+    <t>Rate of natural increase (per 1,000 population)</t>
+  </si>
+  <si>
+    <t>rateofnaturalincreaseper1000population</t>
+  </si>
+  <si>
+    <t>Population change (thousands)</t>
+  </si>
+  <si>
+    <t>PopulationChange</t>
+  </si>
+  <si>
+    <t>Population growth rate (percentage)</t>
+  </si>
+  <si>
+    <t>Total population annual doubling time [n=(ln(2)/r] (years)</t>
+  </si>
+  <si>
+    <t>TotalPopulationAnnualDoubleTime</t>
+  </si>
+  <si>
+    <t>DemographyFormat</t>
+  </si>
+  <si>
+    <t>Alive between birth and age 1</t>
+  </si>
+  <si>
+    <t>Population under age 2</t>
+  </si>
+  <si>
+    <t>Population under age 5</t>
+  </si>
+  <si>
+    <t>Population under age 15</t>
+  </si>
+  <si>
+    <t>Population under age 18</t>
+  </si>
+  <si>
+    <t>Population under age 20</t>
+  </si>
+  <si>
+    <t>Population under age 25</t>
+  </si>
+  <si>
+    <t>Population aged 3-4</t>
+  </si>
+  <si>
+    <t>Population aged 3-5</t>
+  </si>
+  <si>
+    <t>Population aged 3-6</t>
+  </si>
+  <si>
+    <t>Population aged 4-5</t>
+  </si>
+  <si>
+    <t>Population aged 4-6</t>
+  </si>
+  <si>
+    <t>Population aged 5-14</t>
+  </si>
+  <si>
+    <t>Population aged 5-10</t>
+  </si>
+  <si>
+    <t>Population aged 5-11</t>
+  </si>
+  <si>
+    <t>Population aged 6-9</t>
+  </si>
+  <si>
+    <t>Population aged 6-10</t>
+  </si>
+  <si>
+    <t>Population aged 6-11</t>
+  </si>
+  <si>
+    <t>Population aged 6-12</t>
+  </si>
+  <si>
+    <t>Population aged 7-10</t>
+  </si>
+  <si>
+    <t>Population aged 7-12</t>
+  </si>
+  <si>
+    <t>Population aged 11-16</t>
+  </si>
+  <si>
+    <t>Population aged 11-17</t>
+  </si>
+  <si>
+    <t>Population aged 11-18</t>
+  </si>
+  <si>
+    <t>Population aged 12-14</t>
+  </si>
+  <si>
+    <t>Population aged 12-16</t>
+  </si>
+  <si>
+    <t>Population aged 12-17</t>
+  </si>
+  <si>
+    <t>Population aged 12-18</t>
+  </si>
+  <si>
+    <t>Population aged 13-17</t>
+  </si>
+  <si>
+    <t>Population aged 13-18</t>
+  </si>
+  <si>
+    <t>Population aged 13-19</t>
+  </si>
+  <si>
+    <t>Population aged 15-17</t>
+  </si>
+  <si>
+    <t>Population aged 18-23</t>
+  </si>
+  <si>
+    <t>Population aged 15-24</t>
+  </si>
+  <si>
+    <t>Population aged 15-49</t>
+  </si>
+  <si>
+    <t>Population aged 15-59</t>
+  </si>
+  <si>
+    <t>Population aged 15-64</t>
+  </si>
+  <si>
+    <t>Population aged 20-64</t>
+  </si>
+  <si>
+    <t>Population aged 20-69</t>
+  </si>
+  <si>
+    <t>Population aged 25-49</t>
+  </si>
+  <si>
+    <t>Population aged 25-64</t>
+  </si>
+  <si>
+    <t>Population aged 25-69</t>
+  </si>
+  <si>
+    <t>Population aged 15 or over</t>
+  </si>
+  <si>
+    <t>Population aged 16 or over</t>
+  </si>
+  <si>
+    <t>Population aged 17 or over</t>
+  </si>
+  <si>
+    <t>Population aged 18 or over</t>
+  </si>
+  <si>
+    <t>Population aged 20 or over</t>
+  </si>
+  <si>
+    <t>Population aged 21 or over</t>
+  </si>
+  <si>
+    <t>Population aged 25 or over</t>
+  </si>
+  <si>
+    <t>Population aged 50 or over</t>
+  </si>
+  <si>
+    <t>Population aged 60 or over</t>
+  </si>
+  <si>
+    <t>Population aged 65 or over</t>
+  </si>
+  <si>
+    <t>Population aged 70 or over</t>
+  </si>
+  <si>
+    <t>Population aged 75 or over</t>
+  </si>
+  <si>
+    <t>Population aged 80 or over</t>
+  </si>
+  <si>
+    <t>Population aged 85 or over</t>
+  </si>
+  <si>
+    <t>Population aged 90 or over</t>
+  </si>
+  <si>
+    <t>BroadAgeOld</t>
+  </si>
+  <si>
+    <t>BroadAgeNew</t>
+  </si>
+  <si>
+    <t>0_1</t>
+  </si>
+  <si>
+    <t>0_4</t>
+  </si>
+  <si>
+    <t>0_14</t>
+  </si>
+  <si>
+    <t>0_17</t>
+  </si>
+  <si>
+    <t>0_19</t>
+  </si>
+  <si>
+    <t>0_24</t>
+  </si>
+  <si>
+    <t>3_4</t>
+  </si>
+  <si>
+    <t>3_5</t>
+  </si>
+  <si>
+    <t>3_6</t>
+  </si>
+  <si>
+    <t>4_5</t>
+  </si>
+  <si>
+    <t>4_6</t>
+  </si>
+  <si>
+    <t>5_10</t>
+  </si>
+  <si>
+    <t>5_11</t>
+  </si>
+  <si>
+    <t>5_14</t>
+  </si>
+  <si>
+    <t>6_9</t>
+  </si>
+  <si>
+    <t>6_10</t>
+  </si>
+  <si>
+    <t>6_11</t>
+  </si>
+  <si>
+    <t>6_12</t>
+  </si>
+  <si>
+    <t>7_10</t>
+  </si>
+  <si>
+    <t>7_12</t>
+  </si>
+  <si>
+    <t>11_16</t>
+  </si>
+  <si>
+    <t>11_17</t>
+  </si>
+  <si>
+    <t>11_18</t>
+  </si>
+  <si>
+    <t>12_14</t>
+  </si>
+  <si>
+    <t>12_16</t>
+  </si>
+  <si>
+    <t>12_17</t>
+  </si>
+  <si>
+    <t>12_18</t>
+  </si>
+  <si>
+    <t>13_17</t>
+  </si>
+  <si>
+    <t>13_18</t>
+  </si>
+  <si>
+    <t>13_19</t>
+  </si>
+  <si>
+    <t>15plus</t>
+  </si>
+  <si>
+    <t>15_17</t>
+  </si>
+  <si>
+    <t>15_24</t>
+  </si>
+  <si>
+    <t>15_49</t>
+  </si>
+  <si>
+    <t>15_59</t>
+  </si>
+  <si>
+    <t>15_64</t>
+  </si>
+  <si>
+    <t>16plus</t>
+  </si>
+  <si>
+    <t>17plus</t>
+  </si>
+  <si>
+    <t>18plus</t>
+  </si>
+  <si>
+    <t>18_23</t>
+  </si>
+  <si>
+    <t>20plus</t>
+  </si>
+  <si>
+    <t>20_64</t>
+  </si>
+  <si>
+    <t>20_69</t>
+  </si>
+  <si>
+    <t>21plus</t>
+  </si>
+  <si>
+    <t>25plus</t>
+  </si>
+  <si>
+    <t>25_49</t>
+  </si>
+  <si>
+    <t>25_64</t>
+  </si>
+  <si>
+    <t>25_69</t>
+  </si>
+  <si>
+    <t>50plus</t>
+  </si>
+  <si>
+    <t>60plus</t>
+  </si>
+  <si>
+    <t>65plus</t>
+  </si>
+  <si>
+    <t>70plus</t>
+  </si>
+  <si>
+    <t>75plus</t>
+  </si>
+  <si>
+    <t>80plus</t>
+  </si>
+  <si>
+    <t>85plus</t>
+  </si>
+  <si>
+    <t>90plus</t>
+  </si>
+  <si>
+    <t>WPP2015_INT_F02B_3_ANNUAL_POPULATION_INDICATORS_PERCENTAGE_FEMALE.XLS;WPP2015_INT_F02B_2_ANNUAL_POPULATION_INDICATORS_PERCENTAGE_MALE.XLS</t>
+  </si>
+  <si>
+    <t>BroadAgeFormat</t>
+  </si>
+  <si>
+    <t>OtherFiles</t>
+  </si>
+  <si>
+    <t>WPP2015_INT_F02B_1_ANNUAL_POPULATION_INDICATORS_PERCENTAGE_BOTH_SEXES.XLS</t>
+  </si>
+  <si>
+    <t>WPP2015_INT_F02A_1_ANNUAL_POPULATION_INDICATORS_BOTH_SEXES.XLS</t>
+  </si>
+  <si>
+    <t>WPP2015_INT_F02A_3_ANNUAL_POPULATION_INDICATORS_FEMALE.XLS;WPP2015_INT_F02A_2_ANNUAL_POPULATION_INDICATORS_MALE.XLS</t>
+  </si>
+  <si>
+    <t>Annual total dep. ratio [(0-14 &amp; 65+) / 15-64] (%)</t>
+  </si>
+  <si>
+    <t>Annual total dep. ratio [(0-19 &amp; 65+) / 20-64] (%)</t>
+  </si>
+  <si>
+    <t>Annual total dep. ratio [(0-19 &amp; 70+) / 20-69] (%)</t>
+  </si>
+  <si>
+    <t>Annual total dep. ratio [(0-24 &amp; 65+) / 25-64] (%)</t>
+  </si>
+  <si>
+    <t>Annual total dep. ratio [(0-24 &amp; 70+) / 25-69] (%)</t>
+  </si>
+  <si>
+    <t>Annual child dep. ratio [0-14 / 15-64] (%)</t>
+  </si>
+  <si>
+    <t>Annual child dep. ratio [0-19 / 20-64] (%)</t>
+  </si>
+  <si>
+    <t>Annual child dep. ratio [0-19 / 20-69] (%)</t>
+  </si>
+  <si>
+    <t>Annual child dep. ratio [0-24 / 25-69] (%)</t>
+  </si>
+  <si>
+    <t>Annual child dep. ratio [0-24 / 25-64] (%)</t>
+  </si>
+  <si>
+    <t>Annual old-age dep. ratio [65+ / 15-64] (%)</t>
+  </si>
+  <si>
+    <t>Annual old-age dep. ratio [65+ / 20-64] (%)</t>
+  </si>
+  <si>
+    <t>Annual old-age dep. ratio [70+ / 20-69] (%)</t>
+  </si>
+  <si>
+    <t>Annual old-age dep. ratio [70+ / 25-69] (%)</t>
+  </si>
+  <si>
+    <t>Annual old-age dep. ratio [65+ / 25-64] (%)</t>
+  </si>
+  <si>
+    <t>Annual potential support ratio [15-64/65+]</t>
+  </si>
+  <si>
+    <t>Annual potential support ratio [20-64/65+]</t>
+  </si>
+  <si>
+    <t>Annual potential support ratio [20-69/70+]</t>
+  </si>
+  <si>
+    <t>Annual potential support ratio [25-69/70+]</t>
+  </si>
+  <si>
+    <t>Annual potential support ratio [25-64/65+]</t>
+  </si>
+  <si>
+    <t>DependencyOld</t>
+  </si>
+  <si>
+    <t>DependencyNew</t>
+  </si>
+  <si>
+    <t>DepenndencyExtraFiles</t>
+  </si>
+  <si>
+    <t>WPP2015_INT_F02C_1_ANNUAL_POPULATION_INDICATORS_DEPENDENCY_RATIOS_BOTH_SEXES.XLS</t>
+  </si>
+  <si>
+    <t>WPP2015_INT_F02C_2_ANNUAL_POPULATION_INDICATORS_DEPENDENCY_RATIOS_MALE.XLS;WPP2015_INT_F02C_3_ANNUAL_POPULATION_INDICATORS_DEPENDENCY_RATIOS_FEMALE.XLS</t>
+  </si>
+  <si>
+    <t>DependencyFormat</t>
   </si>
 </sst>
 </file>
@@ -755,7 +1295,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -768,6 +1308,18 @@
         <bgColor rgb="FF000000"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -778,23 +1330,33 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="5">
+  <cellStyleXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="5">
+  <cellStyles count="9">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1070,21 +1632,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F81"/>
+  <dimension ref="A1:G87"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A47" workbookViewId="0">
-      <selection activeCell="E75" sqref="E75"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A54" sqref="A54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="125.33203125" customWidth="1"/>
+    <col min="1" max="1" width="127.6640625" customWidth="1"/>
     <col min="2" max="2" width="37.83203125" customWidth="1"/>
-    <col min="4" max="4" width="35.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="83" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.6640625" customWidth="1"/>
+    <col min="5" max="5" width="20.1640625" customWidth="1"/>
+    <col min="7" max="7" width="166.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1103,8 +1666,11 @@
       <c r="F1" s="1" t="s">
         <v>225</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G1" s="1" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>5</v>
       </c>
@@ -1124,8 +1690,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A3" s="1" t="s">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A3" s="3" t="s">
         <v>10</v>
       </c>
       <c r="B3" s="1" t="s">
@@ -1141,11 +1707,11 @@
         <v>13</v>
       </c>
       <c r="F3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A4" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A4" s="3" t="s">
         <v>14</v>
       </c>
       <c r="B4" s="1" t="s">
@@ -1161,11 +1727,11 @@
         <v>16</v>
       </c>
       <c r="F4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A5" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A5" s="3" t="s">
         <v>17</v>
       </c>
       <c r="B5" s="1" t="s">
@@ -1181,11 +1747,11 @@
         <v>19</v>
       </c>
       <c r="F5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A6" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A6" s="3" t="s">
         <v>20</v>
       </c>
       <c r="B6" s="1" t="s">
@@ -1201,11 +1767,11 @@
         <v>22</v>
       </c>
       <c r="F6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A7" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A7" s="3" t="s">
         <v>23</v>
       </c>
       <c r="B7" s="1" t="s">
@@ -1221,10 +1787,10 @@
         <v>25</v>
       </c>
       <c r="F7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>26</v>
       </c>
@@ -1244,8 +1810,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A9" s="1" t="s">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A9" s="3" t="s">
         <v>29</v>
       </c>
       <c r="B9" s="1" t="s">
@@ -1261,11 +1827,11 @@
         <v>31</v>
       </c>
       <c r="F9">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A10" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A10" s="3" t="s">
         <v>32</v>
       </c>
       <c r="B10" s="1" t="s">
@@ -1281,11 +1847,11 @@
         <v>34</v>
       </c>
       <c r="F10">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A11" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A11" s="3" t="s">
         <v>35</v>
       </c>
       <c r="B11" s="1" t="s">
@@ -1301,11 +1867,11 @@
         <v>37</v>
       </c>
       <c r="F11">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A12" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A12" s="3" t="s">
         <v>38</v>
       </c>
       <c r="B12" s="1" t="s">
@@ -1321,11 +1887,11 @@
         <v>40</v>
       </c>
       <c r="F12">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A13" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A13" s="3" t="s">
         <v>41</v>
       </c>
       <c r="B13" s="1" t="s">
@@ -1341,10 +1907,10 @@
         <v>43</v>
       </c>
       <c r="F13">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>44</v>
       </c>
@@ -1364,7 +1930,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>48</v>
       </c>
@@ -1384,7 +1950,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>52</v>
       </c>
@@ -1825,7 +2391,7 @@
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A38" s="1" t="s">
+      <c r="A38" s="3" t="s">
         <v>114</v>
       </c>
       <c r="B38" s="1" t="s">
@@ -1841,11 +2407,11 @@
         <v>116</v>
       </c>
       <c r="F38">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A39" s="1" t="s">
+      <c r="A39" s="3" t="s">
         <v>117</v>
       </c>
       <c r="B39" s="1" t="s">
@@ -1861,11 +2427,11 @@
         <v>119</v>
       </c>
       <c r="F39">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A40" s="1" t="s">
+      <c r="A40" s="3" t="s">
         <v>120</v>
       </c>
       <c r="B40" s="1" t="s">
@@ -1881,11 +2447,11 @@
         <v>122</v>
       </c>
       <c r="F40">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A41" s="1" t="s">
+      <c r="A41" s="3" t="s">
         <v>123</v>
       </c>
       <c r="B41" s="1" t="s">
@@ -1901,11 +2467,11 @@
         <v>125</v>
       </c>
       <c r="F41">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A42" s="1" t="s">
+      <c r="A42" s="3" t="s">
         <v>126</v>
       </c>
       <c r="B42" s="1" t="s">
@@ -1921,7 +2487,7 @@
         <v>128</v>
       </c>
       <c r="F42">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.2">
@@ -1965,11 +2531,11 @@
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A45" s="1" t="s">
+      <c r="A45" s="3" t="s">
         <v>134</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>45</v>
+        <v>145</v>
       </c>
       <c r="C45" s="2" t="s">
         <v>57</v>
@@ -1981,15 +2547,15 @@
         <v>136</v>
       </c>
       <c r="F45">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A46" s="1" t="s">
+      <c r="A46" s="3" t="s">
         <v>137</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>45</v>
+        <v>145</v>
       </c>
       <c r="C46" s="1" t="s">
         <v>61</v>
@@ -2001,7 +2567,7 @@
         <v>138</v>
       </c>
       <c r="F46">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.2">
@@ -2045,7 +2611,7 @@
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A49" s="1" t="s">
+      <c r="A49" s="4" t="s">
         <v>144</v>
       </c>
       <c r="B49" s="1" t="s">
@@ -2061,7 +2627,7 @@
         <v>146</v>
       </c>
       <c r="F49">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.2">
@@ -2125,11 +2691,11 @@
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A53" s="1" t="s">
+      <c r="A53" s="3" t="s">
         <v>153</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>45</v>
+        <v>145</v>
       </c>
       <c r="C53" s="1" t="s">
         <v>53</v>
@@ -2141,11 +2707,11 @@
         <v>154</v>
       </c>
       <c r="F53">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A54" s="1" t="s">
+      <c r="A54" s="4" t="s">
         <v>155</v>
       </c>
       <c r="B54" s="1" t="s">
@@ -2161,7 +2727,7 @@
         <v>156</v>
       </c>
       <c r="F54">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.2">
@@ -2183,11 +2749,11 @@
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A56" s="1" t="s">
+      <c r="A56" s="3" t="s">
         <v>159</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>45</v>
+        <v>145</v>
       </c>
       <c r="C56" s="2"/>
       <c r="D56" s="1" t="s">
@@ -2197,7 +2763,7 @@
         <v>160</v>
       </c>
       <c r="F56">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.2">
@@ -2241,7 +2807,7 @@
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A59" s="1" t="s">
+      <c r="A59" s="3" t="s">
         <v>167</v>
       </c>
       <c r="B59" s="1" t="s">
@@ -2257,11 +2823,11 @@
         <v>169</v>
       </c>
       <c r="F59">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A60" s="1" t="s">
+      <c r="A60" s="3" t="s">
         <v>170</v>
       </c>
       <c r="B60" s="1" t="s">
@@ -2277,11 +2843,11 @@
         <v>172</v>
       </c>
       <c r="F60">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A61" s="1" t="s">
+      <c r="A61" s="3" t="s">
         <v>173</v>
       </c>
       <c r="B61" s="1" t="s">
@@ -2297,11 +2863,11 @@
         <v>175</v>
       </c>
       <c r="F61">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A62" s="1" t="s">
+      <c r="A62" s="3" t="s">
         <v>176</v>
       </c>
       <c r="B62" s="1" t="s">
@@ -2317,11 +2883,11 @@
         <v>178</v>
       </c>
       <c r="F62">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A63" s="1" t="s">
+      <c r="A63" s="3" t="s">
         <v>179</v>
       </c>
       <c r="B63" s="1" t="s">
@@ -2337,7 +2903,7 @@
         <v>181</v>
       </c>
       <c r="F63">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.2">
@@ -2678,12 +3244,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A81" s="1" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="B81" s="1" t="s">
-        <v>226</v>
+        <v>260</v>
       </c>
       <c r="C81" s="1" t="s">
         <v>7</v>
@@ -2692,10 +3258,1103 @@
         <v>226</v>
       </c>
       <c r="E81" t="s">
-        <v>227</v>
+        <v>232</v>
       </c>
       <c r="F81">
         <v>1</v>
+      </c>
+    </row>
+    <row r="82" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A82" s="1" t="s">
+        <v>405</v>
+      </c>
+      <c r="B82" s="1" t="s">
+        <v>407</v>
+      </c>
+      <c r="C82" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D82" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="E82" t="s">
+        <v>232</v>
+      </c>
+      <c r="F82">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="83" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A83" s="1" t="s">
+        <v>406</v>
+      </c>
+      <c r="B83" s="1" t="s">
+        <v>407</v>
+      </c>
+      <c r="C83" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D83" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="E83" t="s">
+        <v>234</v>
+      </c>
+      <c r="F83">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="84" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A84" t="s">
+        <v>376</v>
+      </c>
+      <c r="B84" s="1" t="s">
+        <v>377</v>
+      </c>
+      <c r="C84" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D84" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="E84" t="s">
+        <v>136</v>
+      </c>
+      <c r="F84">
+        <v>1</v>
+      </c>
+      <c r="G84" s="1" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="85" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A85" t="s">
+        <v>379</v>
+      </c>
+      <c r="B85" s="1" t="s">
+        <v>377</v>
+      </c>
+      <c r="C85" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D85" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="E85" t="s">
+        <v>138</v>
+      </c>
+      <c r="F85">
+        <v>1</v>
+      </c>
+      <c r="G85" s="1" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="86" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A86" t="s">
+        <v>381</v>
+      </c>
+      <c r="B86" s="1" t="s">
+        <v>377</v>
+      </c>
+      <c r="C86" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D86" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="E86" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="F86">
+        <v>1</v>
+      </c>
+      <c r="G86" s="1" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="87" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A87" t="s">
+        <v>380</v>
+      </c>
+      <c r="B87" s="1" t="s">
+        <v>377</v>
+      </c>
+      <c r="C87" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D87" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="E87" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="F87">
+        <v>1</v>
+      </c>
+      <c r="G87" s="1" t="s">
+        <v>153</v>
+      </c>
+    </row>
+  </sheetData>
+  <autoFilter ref="A1:G87"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C18"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C24" sqref="C24"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="64.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="34.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="59.5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>228</v>
+      </c>
+      <c r="B1" t="s">
+        <v>229</v>
+      </c>
+      <c r="C1" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>231</v>
+      </c>
+      <c r="B2" t="s">
+        <v>199</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>233</v>
+      </c>
+      <c r="B3" t="s">
+        <v>199</v>
+      </c>
+      <c r="C3" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>235</v>
+      </c>
+      <c r="B4" t="s">
+        <v>236</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>237</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>238</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="C6" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>239</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>240</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>241</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>242</v>
+      </c>
+      <c r="B9" t="s">
+        <v>243</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>244</v>
+      </c>
+      <c r="B10" t="s">
+        <v>245</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>246</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>247</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>248</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>249</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>250</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>210</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>251</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>252</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>253</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>254</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>255</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>256</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>257</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>258</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>259</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>232</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B59"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="25.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>318</v>
+      </c>
+      <c r="B1" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>261</v>
+      </c>
+      <c r="B2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>262</v>
+      </c>
+      <c r="B3" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>263</v>
+      </c>
+      <c r="B4" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>264</v>
+      </c>
+      <c r="B5" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>265</v>
+      </c>
+      <c r="B6" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>266</v>
+      </c>
+      <c r="B7" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>267</v>
+      </c>
+      <c r="B8" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>268</v>
+      </c>
+      <c r="B9" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>269</v>
+      </c>
+      <c r="B10" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>270</v>
+      </c>
+      <c r="B11" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>271</v>
+      </c>
+      <c r="B12" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>272</v>
+      </c>
+      <c r="B13" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>273</v>
+      </c>
+      <c r="B14" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>274</v>
+      </c>
+      <c r="B15" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>275</v>
+      </c>
+      <c r="B16" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>276</v>
+      </c>
+      <c r="B17" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>277</v>
+      </c>
+      <c r="B18" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>278</v>
+      </c>
+      <c r="B19" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>279</v>
+      </c>
+      <c r="B20" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>280</v>
+      </c>
+      <c r="B21" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>281</v>
+      </c>
+      <c r="B22" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>282</v>
+      </c>
+      <c r="B23" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>283</v>
+      </c>
+      <c r="B24" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>284</v>
+      </c>
+      <c r="B25" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>285</v>
+      </c>
+      <c r="B26" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>286</v>
+      </c>
+      <c r="B27" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>287</v>
+      </c>
+      <c r="B28" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>288</v>
+      </c>
+      <c r="B29" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>289</v>
+      </c>
+      <c r="B30" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>290</v>
+      </c>
+      <c r="B31" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>291</v>
+      </c>
+      <c r="B32" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>292</v>
+      </c>
+      <c r="B33" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>293</v>
+      </c>
+      <c r="B34" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>294</v>
+      </c>
+      <c r="B35" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>295</v>
+      </c>
+      <c r="B36" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>296</v>
+      </c>
+      <c r="B37" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
+        <v>297</v>
+      </c>
+      <c r="B38" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
+        <v>298</v>
+      </c>
+      <c r="B39" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
+        <v>299</v>
+      </c>
+      <c r="B40" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
+        <v>300</v>
+      </c>
+      <c r="B41" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
+        <v>301</v>
+      </c>
+      <c r="B42" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
+        <v>302</v>
+      </c>
+      <c r="B43" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A44" t="s">
+        <v>303</v>
+      </c>
+      <c r="B44" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A45" t="s">
+        <v>304</v>
+      </c>
+      <c r="B45" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A46" t="s">
+        <v>305</v>
+      </c>
+      <c r="B46" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A47" t="s">
+        <v>306</v>
+      </c>
+      <c r="B47" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A48" t="s">
+        <v>307</v>
+      </c>
+      <c r="B48" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A49" t="s">
+        <v>308</v>
+      </c>
+      <c r="B49" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A50" t="s">
+        <v>309</v>
+      </c>
+      <c r="B50" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A51" t="s">
+        <v>310</v>
+      </c>
+      <c r="B51" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A52" t="s">
+        <v>311</v>
+      </c>
+      <c r="B52" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A53" t="s">
+        <v>312</v>
+      </c>
+      <c r="B53" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A54" t="s">
+        <v>313</v>
+      </c>
+      <c r="B54" t="s">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A55" t="s">
+        <v>314</v>
+      </c>
+      <c r="B55" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A56" t="s">
+        <v>315</v>
+      </c>
+      <c r="B56" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A57" t="s">
+        <v>316</v>
+      </c>
+      <c r="B57" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A58" t="s">
+        <v>317</v>
+      </c>
+      <c r="B58" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A59" t="s">
+        <v>53</v>
+      </c>
+      <c r="B59" t="s">
+        <v>61</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C21"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F12" sqref="F12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="40.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="55.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>402</v>
+      </c>
+      <c r="B1" t="s">
+        <v>403</v>
+      </c>
+      <c r="C1" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>382</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>383</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>384</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>385</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>386</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>387</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>388</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>389</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>390</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>391</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>392</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>393</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>394</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>395</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>396</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>397</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>398</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>399</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>400</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>401</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>179</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fixed variant uppercase issue & produced datapackage.json file
</commit_message>
<xml_diff>
--- a/etl/source/metadata.xlsx
+++ b/etl/source/metadata.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/Data/GapMinder/testWorkDir/etl/source/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/Data/GapMinder/ddf--unpop--wpp_population/etl/source/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -1634,15 +1634,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G87"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A54" sqref="A54"/>
+    <sheetView tabSelected="1" topLeftCell="A45" workbookViewId="0">
+      <selection activeCell="G61" sqref="G61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="127.6640625" customWidth="1"/>
     <col min="2" max="2" width="37.83203125" customWidth="1"/>
-    <col min="4" max="4" width="18.6640625" customWidth="1"/>
+    <col min="4" max="4" width="35.33203125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="20.1640625" customWidth="1"/>
     <col min="7" max="7" width="166.6640625" bestFit="1" customWidth="1"/>
   </cols>

</xml_diff>